<commit_message>
update VN Fuel 20210506
</commit_message>
<xml_diff>
--- a/Vietnam_Fuel_Price.xlsx
+++ b/Vietnam_Fuel_Price.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dsvcorp-my.sharepoint.com/personal/phuong_ngo_vn_dsv_com/Documents/HP Working Folder/03. Reporting/00. Data for Reporting/01. Fuel Price/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Phuong.Ngo\Documents\GitHub\DSV_Dataset_Fuel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="267" documentId="8_{6FC66A8C-8B36-4CEE-AE76-32B3FB4DDB3F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4DA6E979-4DEB-4F98-A560-F5D48CDAD981}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F66AF8A-5A71-4626-8D2C-BE81D1BF036E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{34EAE4CE-5004-40BE-891B-11B587969404}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28095" windowHeight="16440" xr2:uid="{34EAE4CE-5004-40BE-891B-11B587969404}"/>
   </bookViews>
   <sheets>
     <sheet name="Vietnam_Fuel_Price_CSV" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
     <author>Phuong Ngo - DSV</author>
   </authors>
   <commentList>
-    <comment ref="B116" authorId="0" shapeId="0" xr:uid="{622CD47E-42DA-4105-A1A5-9DF50FA9AFBC}">
+    <comment ref="B124" authorId="0" shapeId="0" xr:uid="{622CD47E-42DA-4105-A1A5-9DF50FA9AFBC}">
       <text>
         <r>
           <rPr>
@@ -46,7 +46,8 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
+            <charset val="163"/>
           </rPr>
           <t>Phuong Ngo - DSV:</t>
         </r>
@@ -55,7 +56,8 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
+            <charset val="163"/>
           </rPr>
           <t xml:space="preserve">
 Petrolimex doesnot post the DO price update on 22 Oct 2018 on their website</t>
@@ -67,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="9">
   <si>
     <t>Vùng 1</t>
   </si>
@@ -115,14 +117,16 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
+      <charset val="163"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
+      <charset val="163"/>
     </font>
   </fonts>
   <fills count="2">
@@ -165,10 +169,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -468,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1B6A3FE-EFAB-4DA1-8BA4-55B73A73877F}">
-  <dimension ref="B1:H123"/>
+  <dimension ref="B1:H131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
-      <selection activeCell="E115" sqref="E115"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -514,2877 +514,3061 @@
     </row>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2" s="1">
-        <v>44252</v>
+        <v>44313</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
       </c>
       <c r="D2">
-        <v>18180</v>
+        <v>19260</v>
       </c>
       <c r="E2">
-        <v>18080</v>
+        <v>19160</v>
       </c>
       <c r="F2">
-        <v>17030</v>
+        <v>17980</v>
       </c>
       <c r="G2">
-        <v>14190</v>
+        <v>14670</v>
       </c>
       <c r="H2">
-        <v>13840</v>
+        <v>14320</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" s="1">
-        <v>44252</v>
+        <v>44313</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
       </c>
       <c r="D3">
-        <v>18540</v>
+        <v>19640</v>
       </c>
       <c r="E3">
-        <v>18440</v>
+        <v>19540</v>
       </c>
       <c r="F3">
-        <v>17370</v>
+        <v>18330</v>
       </c>
       <c r="G3">
-        <v>14470</v>
+        <v>14960</v>
       </c>
       <c r="H3">
-        <v>14110</v>
+        <v>14600</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
-        <v>44237</v>
+        <v>44298</v>
       </c>
       <c r="C4" t="s">
         <v>0</v>
       </c>
       <c r="D4">
-        <v>17370</v>
+        <v>19070</v>
       </c>
       <c r="E4">
-        <v>17270</v>
+        <v>18970</v>
       </c>
       <c r="F4">
-        <v>16300</v>
+        <v>17800</v>
       </c>
       <c r="G4">
-        <v>13390</v>
+        <v>14490</v>
       </c>
       <c r="H4">
-        <v>13040</v>
+        <v>14140</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
-        <v>44237</v>
+        <v>44298</v>
       </c>
       <c r="C5" t="s">
         <v>1</v>
       </c>
       <c r="D5">
-        <v>17710</v>
+        <v>19450</v>
       </c>
       <c r="E5">
-        <v>17610</v>
+        <v>19340</v>
       </c>
       <c r="F5">
-        <v>16620</v>
+        <v>18150</v>
       </c>
       <c r="G5">
-        <v>13650</v>
+        <v>14770</v>
       </c>
       <c r="H5">
-        <v>13300</v>
+        <v>14420</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
-        <v>44222</v>
+        <v>44282</v>
       </c>
       <c r="C6" t="s">
         <v>0</v>
       </c>
       <c r="D6">
-        <v>17370</v>
+        <v>19140</v>
       </c>
       <c r="E6">
-        <v>17270</v>
+        <v>19040</v>
       </c>
       <c r="F6">
-        <v>16300</v>
+        <v>17850</v>
       </c>
       <c r="G6">
-        <v>13390</v>
+        <v>14590</v>
       </c>
       <c r="H6">
-        <v>13040</v>
+        <v>14240</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
-        <v>44222</v>
+        <v>44282</v>
       </c>
       <c r="C7" t="s">
         <v>1</v>
       </c>
       <c r="D7">
-        <v>17710</v>
+        <v>19520</v>
       </c>
       <c r="E7">
-        <v>17610</v>
+        <v>19420</v>
       </c>
       <c r="F7">
-        <v>16620</v>
+        <v>18200</v>
       </c>
       <c r="G7">
-        <v>13650</v>
+        <v>14880</v>
       </c>
       <c r="H7">
-        <v>13300</v>
+        <v>14520</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
-        <v>44207</v>
+        <v>44267</v>
       </c>
       <c r="C8" t="s">
         <v>0</v>
       </c>
       <c r="D8">
-        <v>17030</v>
+        <v>18980</v>
       </c>
       <c r="E8">
-        <v>16930</v>
+        <v>18880</v>
       </c>
       <c r="F8">
-        <v>15940</v>
+        <v>17720</v>
       </c>
       <c r="G8">
-        <v>12990</v>
+        <v>14750</v>
       </c>
       <c r="H8">
-        <v>12640</v>
+        <v>14400</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
-        <v>44207</v>
+        <v>44267</v>
       </c>
       <c r="C9" t="s">
         <v>1</v>
       </c>
       <c r="D9">
-        <v>17370</v>
+        <v>19350</v>
       </c>
       <c r="E9">
-        <v>17260</v>
+        <v>19250</v>
       </c>
       <c r="F9">
-        <v>16250</v>
+        <v>18070</v>
       </c>
       <c r="G9">
-        <v>13240</v>
+        <v>15040</v>
       </c>
       <c r="H9">
-        <v>12890</v>
+        <v>14680</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
-        <v>44191</v>
+        <v>44252</v>
       </c>
       <c r="C10" t="s">
         <v>0</v>
       </c>
       <c r="D10">
-        <v>16570</v>
+        <v>18180</v>
       </c>
       <c r="E10">
-        <v>16470</v>
+        <v>18080</v>
       </c>
       <c r="F10">
-        <v>15510</v>
+        <v>17030</v>
       </c>
       <c r="G10">
-        <v>12720</v>
+        <v>14190</v>
       </c>
       <c r="H10">
-        <v>12370</v>
+        <v>13840</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
-        <v>44191</v>
+        <v>44252</v>
       </c>
       <c r="C11" t="s">
         <v>1</v>
       </c>
       <c r="D11">
-        <v>16900</v>
+        <v>18540</v>
       </c>
       <c r="E11">
-        <v>16790</v>
+        <v>18440</v>
       </c>
       <c r="F11">
-        <v>15820</v>
+        <v>17370</v>
       </c>
       <c r="G11">
-        <v>12970</v>
+        <v>14470</v>
       </c>
       <c r="H11">
-        <v>12610</v>
+        <v>14110</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="1">
-        <v>44176</v>
+        <v>44237</v>
       </c>
       <c r="C12" t="s">
         <v>0</v>
       </c>
       <c r="D12">
-        <v>16100</v>
+        <v>17370</v>
       </c>
       <c r="E12">
-        <v>16000</v>
+        <v>17270</v>
       </c>
       <c r="F12">
-        <v>15120</v>
+        <v>16300</v>
       </c>
       <c r="G12">
-        <v>12240</v>
+        <v>13390</v>
       </c>
       <c r="H12">
-        <v>11890</v>
+        <v>13040</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
-        <v>44176</v>
+        <v>44237</v>
       </c>
       <c r="C13" t="s">
         <v>1</v>
       </c>
       <c r="D13">
-        <v>16420</v>
+        <v>17710</v>
       </c>
       <c r="E13">
-        <v>16320</v>
+        <v>17610</v>
       </c>
       <c r="F13">
-        <v>15420</v>
+        <v>16620</v>
       </c>
       <c r="G13">
-        <v>12480</v>
+        <v>13650</v>
       </c>
       <c r="H13">
-        <v>12120</v>
+        <v>13300</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="1">
-        <v>44161</v>
+        <v>44222</v>
       </c>
       <c r="C14" t="s">
         <v>0</v>
       </c>
       <c r="D14">
-        <v>15450</v>
+        <v>17370</v>
       </c>
       <c r="E14">
-        <v>15350</v>
+        <v>17270</v>
       </c>
       <c r="F14">
-        <v>14490</v>
+        <v>16300</v>
       </c>
       <c r="G14">
-        <v>11780</v>
+        <v>13390</v>
       </c>
       <c r="H14">
-        <v>11430</v>
+        <v>13040</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="1">
-        <v>44161</v>
+        <v>44222</v>
       </c>
       <c r="C15" t="s">
         <v>1</v>
       </c>
       <c r="D15">
-        <v>15750</v>
+        <v>17710</v>
       </c>
       <c r="E15">
-        <v>15650</v>
+        <v>17610</v>
       </c>
       <c r="F15">
-        <v>14770</v>
+        <v>16620</v>
       </c>
       <c r="G15">
-        <v>12010</v>
+        <v>13650</v>
       </c>
       <c r="H15">
-        <v>11650</v>
+        <v>13300</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="1">
-        <v>44146</v>
+        <v>44207</v>
       </c>
       <c r="C16" t="s">
         <v>0</v>
       </c>
       <c r="D16">
-        <v>14800</v>
+        <v>17030</v>
       </c>
       <c r="E16">
-        <v>14700</v>
+        <v>16930</v>
       </c>
       <c r="F16">
-        <v>13880</v>
+        <v>15940</v>
       </c>
       <c r="G16">
-        <v>11180</v>
+        <v>12990</v>
       </c>
       <c r="H16">
-        <v>10830</v>
+        <v>12640</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="1">
-        <v>44146</v>
+        <v>44207</v>
       </c>
       <c r="C17" t="s">
         <v>1</v>
       </c>
       <c r="D17">
-        <v>15090</v>
+        <v>17370</v>
       </c>
       <c r="E17">
-        <v>14990</v>
+        <v>17260</v>
       </c>
       <c r="F17">
-        <v>14150</v>
+        <v>16250</v>
       </c>
       <c r="G17">
-        <v>11400</v>
+        <v>13240</v>
       </c>
       <c r="H17">
-        <v>11040</v>
+        <v>12890</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="1">
-        <v>44131</v>
+        <v>44191</v>
       </c>
       <c r="C18" t="s">
         <v>0</v>
       </c>
       <c r="D18">
-        <v>15040</v>
+        <v>16570</v>
       </c>
       <c r="E18">
-        <v>14940</v>
+        <v>16470</v>
       </c>
       <c r="F18">
-        <v>14100</v>
+        <v>15510</v>
       </c>
       <c r="G18">
-        <v>11560</v>
+        <v>12720</v>
       </c>
       <c r="H18">
-        <v>11210</v>
+        <v>12370</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="1">
-        <v>44131</v>
+        <v>44191</v>
       </c>
       <c r="C19" t="s">
         <v>1</v>
       </c>
       <c r="D19">
-        <v>15340</v>
+        <v>16900</v>
       </c>
       <c r="E19">
-        <v>15230</v>
+        <v>16790</v>
       </c>
       <c r="F19">
-        <v>14380</v>
+        <v>15820</v>
       </c>
       <c r="G19">
-        <v>11790</v>
+        <v>12970</v>
       </c>
       <c r="H19">
-        <v>11430</v>
+        <v>12610</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="1">
-        <v>44116</v>
+        <v>44176</v>
       </c>
       <c r="C20" t="s">
         <v>0</v>
       </c>
       <c r="D20">
-        <v>15220</v>
+        <v>16100</v>
       </c>
       <c r="E20">
+        <v>16000</v>
+      </c>
+      <c r="F20">
         <v>15120</v>
       </c>
-      <c r="F20">
-        <v>14260</v>
-      </c>
       <c r="G20">
-        <v>11470</v>
+        <v>12240</v>
       </c>
       <c r="H20">
-        <v>11120</v>
+        <v>11890</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="1">
-        <v>44116</v>
+        <v>44176</v>
       </c>
       <c r="C21" t="s">
         <v>1</v>
       </c>
       <c r="D21">
-        <v>15520</v>
+        <v>16420</v>
       </c>
       <c r="E21">
+        <v>16320</v>
+      </c>
+      <c r="F21">
         <v>15420</v>
       </c>
-      <c r="F21">
-        <v>14540</v>
-      </c>
       <c r="G21">
-        <v>11690</v>
+        <v>12480</v>
       </c>
       <c r="H21">
-        <v>11340</v>
+        <v>12120</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="1">
-        <v>44100</v>
+        <v>44161</v>
       </c>
       <c r="C22" t="s">
         <v>0</v>
       </c>
       <c r="D22">
-        <v>15080</v>
+        <v>15450</v>
       </c>
       <c r="E22">
-        <v>14980</v>
+        <v>15350</v>
       </c>
       <c r="F22">
-        <v>14210</v>
+        <v>14490</v>
       </c>
       <c r="G22">
-        <v>11520</v>
+        <v>11780</v>
       </c>
       <c r="H22">
-        <v>11120</v>
+        <v>11430</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="1">
-        <v>44100</v>
+        <v>44161</v>
       </c>
       <c r="C23" t="s">
         <v>1</v>
       </c>
       <c r="D23">
-        <v>15380</v>
+        <v>15750</v>
       </c>
       <c r="E23">
-        <v>15270</v>
+        <v>15650</v>
       </c>
       <c r="F23">
-        <v>14490</v>
+        <v>14770</v>
       </c>
       <c r="G23">
-        <v>11750</v>
+        <v>12010</v>
       </c>
       <c r="H23">
-        <v>11340</v>
+        <v>11650</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="1">
-        <v>44085</v>
+        <v>44146</v>
       </c>
       <c r="C24" t="s">
         <v>0</v>
       </c>
       <c r="D24">
-        <v>15080</v>
+        <v>14800</v>
       </c>
       <c r="E24">
-        <v>14980</v>
+        <v>14700</v>
       </c>
       <c r="F24">
-        <v>14260</v>
+        <v>13880</v>
       </c>
       <c r="G24">
-        <v>11910</v>
+        <v>11180</v>
       </c>
       <c r="H24">
-        <v>11510</v>
+        <v>10830</v>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" s="1">
-        <v>44085</v>
+        <v>44146</v>
       </c>
       <c r="C25" t="s">
         <v>1</v>
       </c>
       <c r="D25">
-        <v>15380</v>
+        <v>15090</v>
       </c>
       <c r="E25">
-        <v>15270</v>
+        <v>14990</v>
       </c>
       <c r="F25">
-        <v>14540</v>
+        <v>14150</v>
       </c>
       <c r="G25">
-        <v>12140</v>
+        <v>11400</v>
       </c>
       <c r="H25">
-        <v>11740</v>
+        <v>11040</v>
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="1">
-        <v>44070</v>
+        <v>44131</v>
       </c>
       <c r="C26" t="s">
         <v>0</v>
       </c>
       <c r="D26">
-        <v>15210</v>
+        <v>15040</v>
       </c>
       <c r="E26">
-        <v>15110</v>
+        <v>14940</v>
       </c>
       <c r="F26">
-        <v>14400</v>
+        <v>14100</v>
       </c>
       <c r="G26">
-        <v>12260</v>
+        <v>11560</v>
       </c>
       <c r="H26">
-        <v>11960</v>
+        <v>11210</v>
       </c>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" s="1">
-        <v>44070</v>
+        <v>44131</v>
       </c>
       <c r="C27" t="s">
         <v>1</v>
       </c>
       <c r="D27">
-        <v>15510</v>
+        <v>15340</v>
       </c>
       <c r="E27">
-        <v>15410</v>
+        <v>15230</v>
       </c>
       <c r="F27">
-        <v>14680</v>
+        <v>14380</v>
       </c>
       <c r="G27">
-        <v>12500</v>
+        <v>11790</v>
       </c>
       <c r="H27">
-        <v>12190</v>
+        <v>11430</v>
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" s="1">
-        <v>44055</v>
+        <v>44116</v>
       </c>
       <c r="C28" t="s">
         <v>0</v>
       </c>
       <c r="D28">
-        <v>15020</v>
+        <v>15220</v>
       </c>
       <c r="E28">
-        <v>14920</v>
+        <v>15120</v>
       </c>
       <c r="F28">
-        <v>14400</v>
+        <v>14260</v>
       </c>
       <c r="G28">
-        <v>12450</v>
+        <v>11470</v>
       </c>
       <c r="H28">
-        <v>12200</v>
+        <v>11120</v>
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B29" s="1">
-        <v>44055</v>
+        <v>44116</v>
       </c>
       <c r="C29" t="s">
         <v>1</v>
       </c>
       <c r="D29">
-        <v>15320</v>
+        <v>15520</v>
       </c>
       <c r="E29">
-        <v>15210</v>
+        <v>15420</v>
       </c>
       <c r="F29">
-        <v>14680</v>
+        <v>14540</v>
       </c>
       <c r="G29">
-        <v>12690</v>
+        <v>11690</v>
       </c>
       <c r="H29">
-        <v>12440</v>
+        <v>11340</v>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B30" s="1">
-        <v>44040</v>
+        <v>44100</v>
       </c>
       <c r="C30" t="s">
         <v>0</v>
       </c>
       <c r="D30">
-        <v>15070</v>
+        <v>15080</v>
       </c>
       <c r="E30">
-        <v>14970</v>
+        <v>14980</v>
       </c>
       <c r="F30">
-        <v>14400</v>
+        <v>14210</v>
       </c>
       <c r="G30">
-        <v>12590</v>
+        <v>11520</v>
       </c>
       <c r="H30">
-        <v>12390</v>
+        <v>11120</v>
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B31" s="1">
-        <v>44040</v>
+        <v>44100</v>
       </c>
       <c r="C31" t="s">
         <v>1</v>
       </c>
       <c r="D31">
-        <v>15370</v>
+        <v>15380</v>
       </c>
       <c r="E31">
-        <v>15260</v>
+        <v>15270</v>
       </c>
       <c r="F31">
-        <v>14680</v>
+        <v>14490</v>
       </c>
       <c r="G31">
-        <v>12840</v>
+        <v>11750</v>
       </c>
       <c r="H31">
-        <v>12630</v>
+        <v>11340</v>
       </c>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B32" s="1">
-        <v>44025</v>
+        <v>44085</v>
       </c>
       <c r="C32" t="s">
         <v>0</v>
       </c>
       <c r="D32">
-        <v>15070</v>
+        <v>15080</v>
       </c>
       <c r="E32">
-        <v>14970</v>
+        <v>14980</v>
       </c>
       <c r="F32">
-        <v>14250</v>
+        <v>14260</v>
       </c>
       <c r="G32">
-        <v>12310</v>
+        <v>11910</v>
       </c>
       <c r="H32">
-        <v>12110</v>
+        <v>11510</v>
       </c>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B33" s="1">
-        <v>44025</v>
+        <v>44085</v>
       </c>
       <c r="C33" t="s">
         <v>1</v>
       </c>
       <c r="D33">
-        <v>15370</v>
+        <v>15380</v>
       </c>
       <c r="E33">
-        <v>15260</v>
+        <v>15270</v>
       </c>
       <c r="F33">
-        <v>14530</v>
+        <v>14540</v>
       </c>
       <c r="G33">
-        <v>12550</v>
+        <v>12140</v>
       </c>
       <c r="H33">
-        <v>12350</v>
+        <v>11740</v>
       </c>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B34" s="1">
-        <v>44009</v>
+        <v>44070</v>
       </c>
       <c r="C34" t="s">
         <v>0</v>
       </c>
       <c r="D34">
-        <v>15070</v>
+        <v>15210</v>
       </c>
       <c r="E34">
-        <v>14970</v>
+        <v>15110</v>
       </c>
       <c r="F34">
-        <v>14250</v>
+        <v>14400</v>
       </c>
       <c r="G34">
-        <v>12410</v>
+        <v>12260</v>
       </c>
       <c r="H34">
-        <v>12110</v>
+        <v>11960</v>
       </c>
     </row>
     <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B35" s="1">
-        <v>44009</v>
+        <v>44070</v>
       </c>
       <c r="C35" t="s">
         <v>1</v>
       </c>
       <c r="D35">
-        <v>15370</v>
+        <v>15510</v>
       </c>
       <c r="E35">
-        <v>15260</v>
+        <v>15410</v>
       </c>
       <c r="F35">
-        <v>14530</v>
+        <v>14680</v>
       </c>
       <c r="G35">
-        <v>12650</v>
+        <v>12500</v>
       </c>
       <c r="H35">
-        <v>12350</v>
+        <v>12190</v>
       </c>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B36" s="1">
-        <f>B34-15</f>
-        <v>43994</v>
+        <v>44055</v>
       </c>
       <c r="C36" t="s">
         <v>0</v>
       </c>
       <c r="D36">
-        <v>14180</v>
+        <v>15020</v>
       </c>
       <c r="E36">
-        <v>14080</v>
+        <v>14920</v>
       </c>
       <c r="F36">
-        <v>13390</v>
+        <v>14400</v>
       </c>
       <c r="G36">
-        <v>11810</v>
+        <v>12450</v>
       </c>
       <c r="H36">
-        <v>11510</v>
+        <v>12200</v>
       </c>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B37" s="1">
-        <f>B35-15</f>
-        <v>43994</v>
+        <v>44055</v>
       </c>
       <c r="C37" t="s">
         <v>1</v>
       </c>
       <c r="D37">
-        <v>14460</v>
+        <v>15320</v>
       </c>
       <c r="E37">
-        <v>14360</v>
+        <v>15210</v>
       </c>
       <c r="F37">
-        <v>13650</v>
+        <v>14680</v>
       </c>
       <c r="G37">
-        <v>12040</v>
+        <v>12690</v>
       </c>
       <c r="H37">
-        <v>11740</v>
+        <v>12440</v>
       </c>
     </row>
     <row r="38" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B38" s="1">
-        <f t="shared" ref="B38:B47" si="0">B36-15</f>
-        <v>43979</v>
+        <v>44040</v>
       </c>
       <c r="C38" t="s">
         <v>0</v>
       </c>
       <c r="D38">
-        <v>13220</v>
+        <v>15070</v>
       </c>
       <c r="E38">
-        <v>13120</v>
+        <v>14970</v>
       </c>
       <c r="F38">
-        <v>12400</v>
+        <v>14400</v>
       </c>
       <c r="G38">
-        <v>11040</v>
+        <v>12590</v>
       </c>
       <c r="H38">
-        <v>10740</v>
+        <v>12390</v>
       </c>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B39" s="1">
-        <f t="shared" si="0"/>
-        <v>43979</v>
+        <v>44040</v>
       </c>
       <c r="C39" t="s">
         <v>1</v>
       </c>
       <c r="D39">
-        <v>13480</v>
+        <v>15370</v>
       </c>
       <c r="E39">
-        <v>13380</v>
+        <v>15260</v>
       </c>
       <c r="F39">
-        <v>12640</v>
+        <v>14680</v>
       </c>
       <c r="G39">
-        <v>11260</v>
+        <v>12840</v>
       </c>
       <c r="H39">
-        <v>10950</v>
+        <v>12630</v>
       </c>
     </row>
     <row r="40" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B40" s="1">
-        <f t="shared" si="0"/>
-        <v>43964</v>
+        <v>44025</v>
       </c>
       <c r="C40" t="s">
         <v>0</v>
       </c>
       <c r="D40">
-        <v>12330</v>
+        <v>15070</v>
       </c>
       <c r="E40">
-        <v>12230</v>
+        <v>14970</v>
       </c>
       <c r="F40">
-        <v>11520</v>
+        <v>14250</v>
       </c>
       <c r="G40">
-        <v>10150</v>
+        <v>12310</v>
       </c>
       <c r="H40">
-        <v>9850</v>
+        <v>12110</v>
       </c>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B41" s="1">
-        <f t="shared" si="0"/>
-        <v>43964</v>
+        <v>44025</v>
       </c>
       <c r="C41" t="s">
         <v>1</v>
       </c>
       <c r="D41">
-        <v>12570</v>
+        <v>15370</v>
       </c>
       <c r="E41">
-        <v>12470</v>
+        <v>15260</v>
       </c>
       <c r="F41">
-        <v>11750</v>
+        <v>14530</v>
       </c>
       <c r="G41">
-        <v>10350</v>
+        <v>12550</v>
       </c>
       <c r="H41">
-        <v>10040</v>
+        <v>12350</v>
       </c>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B42" s="1">
-        <f t="shared" si="0"/>
-        <v>43949</v>
+        <v>44009</v>
       </c>
       <c r="C42" t="s">
         <v>0</v>
       </c>
       <c r="D42">
-        <v>11730</v>
+        <v>15070</v>
       </c>
       <c r="E42">
-        <v>11630</v>
+        <v>14970</v>
       </c>
       <c r="F42">
-        <v>10940</v>
+        <v>14250</v>
       </c>
       <c r="G42">
-        <v>10240</v>
+        <v>12410</v>
       </c>
       <c r="H42">
-        <v>9940</v>
+        <v>12110</v>
       </c>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B43" s="1">
-        <f t="shared" si="0"/>
-        <v>43949</v>
+        <v>44009</v>
       </c>
       <c r="C43" t="s">
         <v>1</v>
       </c>
       <c r="D43">
-        <v>11960</v>
+        <v>15370</v>
       </c>
       <c r="E43">
-        <v>11860</v>
+        <v>15260</v>
       </c>
       <c r="F43">
-        <v>11150</v>
+        <v>14530</v>
       </c>
       <c r="G43">
-        <v>10440</v>
+        <v>12650</v>
       </c>
       <c r="H43">
-        <v>10130</v>
+        <v>12350</v>
       </c>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B44" s="1">
-        <f t="shared" si="0"/>
-        <v>43934</v>
+        <f>B42-15</f>
+        <v>43994</v>
       </c>
       <c r="C44" t="s">
         <v>0</v>
       </c>
       <c r="D44">
-        <v>12030</v>
+        <v>14180</v>
       </c>
       <c r="E44">
-        <v>11930</v>
+        <v>14080</v>
       </c>
       <c r="F44">
-        <v>11340</v>
+        <v>13390</v>
       </c>
       <c r="G44">
-        <v>11120</v>
+        <v>11810</v>
       </c>
       <c r="H44">
-        <v>10820</v>
+        <v>11510</v>
       </c>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B45" s="1">
-        <f t="shared" si="0"/>
-        <v>43934</v>
+        <f>B43-15</f>
+        <v>43994</v>
       </c>
       <c r="C45" t="s">
         <v>1</v>
       </c>
       <c r="D45">
-        <v>12270</v>
+        <v>14460</v>
       </c>
       <c r="E45">
-        <v>12160</v>
+        <v>14360</v>
       </c>
       <c r="F45">
-        <v>11560</v>
+        <v>13650</v>
       </c>
       <c r="G45">
-        <v>11340</v>
+        <v>12040</v>
       </c>
       <c r="H45">
-        <v>11030</v>
+        <v>11740</v>
       </c>
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B46" s="1">
-        <f t="shared" si="0"/>
-        <v>43919</v>
+        <f t="shared" ref="B46:B55" si="0">B44-15</f>
+        <v>43979</v>
       </c>
       <c r="C46" t="s">
         <v>0</v>
       </c>
       <c r="D46">
-        <v>12660</v>
+        <v>13220</v>
       </c>
       <c r="E46">
-        <v>12560</v>
+        <v>13120</v>
       </c>
       <c r="F46">
-        <v>11950</v>
+        <v>12400</v>
       </c>
       <c r="G46">
-        <v>11550</v>
+        <v>11040</v>
       </c>
       <c r="H46">
-        <v>11250</v>
+        <v>10740</v>
       </c>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B47" s="1">
         <f t="shared" si="0"/>
-        <v>43919</v>
+        <v>43979</v>
       </c>
       <c r="C47" t="s">
         <v>1</v>
       </c>
       <c r="D47">
-        <v>12910</v>
+        <v>13480</v>
       </c>
       <c r="E47">
-        <v>12810</v>
+        <v>13380</v>
       </c>
       <c r="F47">
-        <v>12180</v>
+        <v>12640</v>
       </c>
       <c r="G47">
-        <v>11780</v>
+        <v>11260</v>
       </c>
       <c r="H47">
-        <v>11470</v>
+        <v>10950</v>
       </c>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B48" s="1">
-        <v>43905</v>
+        <f t="shared" si="0"/>
+        <v>43964</v>
       </c>
       <c r="C48" t="s">
         <v>0</v>
       </c>
       <c r="D48">
-        <v>16910</v>
+        <v>12330</v>
       </c>
       <c r="E48">
-        <v>16810</v>
+        <v>12230</v>
       </c>
       <c r="F48">
-        <v>16050</v>
+        <v>11520</v>
       </c>
       <c r="G48">
-        <v>13330</v>
+        <v>10150</v>
       </c>
       <c r="H48">
-        <v>13030</v>
+        <v>9850</v>
       </c>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B49" s="1">
-        <v>43905</v>
+        <f t="shared" si="0"/>
+        <v>43964</v>
       </c>
       <c r="C49" t="s">
         <v>1</v>
       </c>
       <c r="D49">
-        <v>17240</v>
+        <v>12570</v>
       </c>
       <c r="E49">
-        <v>17140</v>
+        <v>12470</v>
       </c>
       <c r="F49">
-        <v>16370</v>
+        <v>11750</v>
       </c>
       <c r="G49">
-        <v>13590</v>
+        <v>10350</v>
       </c>
       <c r="H49">
-        <v>13290</v>
+        <v>10040</v>
       </c>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B50" s="1">
-        <f>B48-15</f>
-        <v>43890</v>
+        <f t="shared" si="0"/>
+        <v>43949</v>
       </c>
       <c r="C50" t="s">
         <v>0</v>
       </c>
       <c r="D50">
-        <v>19220</v>
+        <v>11730</v>
       </c>
       <c r="E50">
-        <v>19120</v>
+        <v>11630</v>
       </c>
       <c r="F50">
-        <v>18340</v>
+        <v>10940</v>
       </c>
       <c r="G50">
-        <v>15080</v>
+        <v>10240</v>
       </c>
       <c r="H50">
-        <v>14780</v>
+        <v>9940</v>
       </c>
     </row>
     <row r="51" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B51" s="1">
-        <f>B49-15</f>
-        <v>43890</v>
+        <f t="shared" si="0"/>
+        <v>43949</v>
       </c>
       <c r="C51" t="s">
         <v>1</v>
       </c>
       <c r="D51">
-        <v>19600</v>
+        <v>11960</v>
       </c>
       <c r="E51">
-        <v>19500</v>
+        <v>11860</v>
       </c>
       <c r="F51">
-        <v>18700</v>
+        <v>11150</v>
       </c>
       <c r="G51">
-        <v>15380</v>
+        <v>10440</v>
       </c>
       <c r="H51">
-        <v>15070</v>
+        <v>10130</v>
       </c>
     </row>
     <row r="52" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B52" s="1">
-        <f t="shared" ref="B52:B61" si="1">B50-15</f>
-        <v>43875</v>
+        <f t="shared" si="0"/>
+        <v>43934</v>
       </c>
       <c r="C52" t="s">
         <v>0</v>
       </c>
       <c r="D52">
-        <v>19480</v>
+        <v>12030</v>
       </c>
       <c r="E52">
-        <v>19380</v>
+        <v>11930</v>
       </c>
       <c r="F52">
-        <v>18500</v>
+        <v>11340</v>
       </c>
       <c r="G52">
-        <v>15470</v>
+        <v>11120</v>
       </c>
       <c r="H52">
-        <v>15170</v>
+        <v>10820</v>
       </c>
     </row>
     <row r="53" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B53" s="1">
-        <f t="shared" si="1"/>
-        <v>43875</v>
+        <f t="shared" si="0"/>
+        <v>43934</v>
       </c>
       <c r="C53" t="s">
         <v>1</v>
       </c>
       <c r="D53">
-        <v>19860</v>
+        <v>12270</v>
       </c>
       <c r="E53">
-        <v>19760</v>
+        <v>12160</v>
       </c>
       <c r="F53">
-        <v>18870</v>
+        <v>11560</v>
       </c>
       <c r="G53">
-        <v>15770</v>
+        <v>11340</v>
       </c>
       <c r="H53">
-        <v>15470</v>
+        <v>11030</v>
       </c>
     </row>
     <row r="54" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B54" s="1">
-        <f t="shared" si="1"/>
-        <v>43860</v>
+        <f t="shared" si="0"/>
+        <v>43919</v>
       </c>
       <c r="C54" t="s">
         <v>0</v>
       </c>
       <c r="D54">
-        <v>20220</v>
+        <v>12660</v>
       </c>
       <c r="E54">
-        <v>20120</v>
+        <v>12560</v>
       </c>
       <c r="F54">
-        <v>19260</v>
+        <v>11950</v>
       </c>
       <c r="G54">
-        <v>16430</v>
+        <v>11550</v>
       </c>
       <c r="H54">
-        <v>16130</v>
+        <v>11250</v>
       </c>
     </row>
     <row r="55" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B55" s="1">
-        <f t="shared" si="1"/>
-        <v>43860</v>
+        <f t="shared" si="0"/>
+        <v>43919</v>
       </c>
       <c r="C55" t="s">
         <v>1</v>
       </c>
       <c r="D55">
-        <v>20620</v>
+        <v>12910</v>
       </c>
       <c r="E55">
-        <v>20520</v>
+        <v>12810</v>
       </c>
       <c r="F55">
-        <v>19640</v>
+        <v>12180</v>
       </c>
       <c r="G55">
-        <v>16750</v>
+        <v>11780</v>
       </c>
       <c r="H55">
-        <v>16450</v>
+        <v>11470</v>
       </c>
     </row>
     <row r="56" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B56" s="1">
-        <f t="shared" si="1"/>
-        <v>43845</v>
+        <v>43905</v>
       </c>
       <c r="C56" t="s">
         <v>0</v>
       </c>
       <c r="D56">
-        <v>21010</v>
+        <v>16910</v>
       </c>
       <c r="E56">
-        <v>20910</v>
+        <v>16810</v>
       </c>
       <c r="F56">
-        <v>19840</v>
+        <v>16050</v>
       </c>
       <c r="G56">
-        <v>16840</v>
+        <v>13330</v>
       </c>
       <c r="H56">
-        <v>16540</v>
+        <v>13030</v>
       </c>
     </row>
     <row r="57" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B57" s="1">
-        <f t="shared" si="1"/>
-        <v>43845</v>
+        <v>43905</v>
       </c>
       <c r="C57" t="s">
         <v>1</v>
       </c>
       <c r="D57">
-        <v>21430</v>
+        <v>17240</v>
       </c>
       <c r="E57">
-        <v>21320</v>
+        <v>17140</v>
       </c>
       <c r="F57">
-        <v>20230</v>
+        <v>16370</v>
       </c>
       <c r="G57">
-        <v>17170</v>
+        <v>13590</v>
       </c>
       <c r="H57">
-        <v>16870</v>
+        <v>13290</v>
       </c>
     </row>
     <row r="58" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B58" s="1">
-        <f t="shared" si="1"/>
-        <v>43830</v>
+        <f>B56-15</f>
+        <v>43890</v>
       </c>
       <c r="C58" t="s">
         <v>0</v>
       </c>
       <c r="D58">
-        <v>21090</v>
+        <v>19220</v>
       </c>
       <c r="E58">
-        <v>20990</v>
+        <v>19120</v>
       </c>
       <c r="F58">
-        <v>19880</v>
+        <v>18340</v>
       </c>
       <c r="G58">
-        <v>16890</v>
+        <v>15080</v>
       </c>
       <c r="H58">
-        <v>16590</v>
+        <v>14780</v>
       </c>
     </row>
     <row r="59" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B59" s="1">
-        <f t="shared" si="1"/>
-        <v>43830</v>
+        <f>B57-15</f>
+        <v>43890</v>
       </c>
       <c r="C59" t="s">
         <v>1</v>
       </c>
       <c r="D59">
-        <v>21510</v>
+        <v>19600</v>
       </c>
       <c r="E59">
-        <v>21400</v>
+        <v>19500</v>
       </c>
       <c r="F59">
-        <v>20270</v>
+        <v>18700</v>
       </c>
       <c r="G59">
-        <v>17220</v>
+        <v>15380</v>
       </c>
       <c r="H59">
-        <v>16920</v>
+        <v>15070</v>
       </c>
     </row>
     <row r="60" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B60" s="1">
-        <f t="shared" si="1"/>
-        <v>43815</v>
+        <f t="shared" ref="B60:B69" si="1">B58-15</f>
+        <v>43875</v>
       </c>
       <c r="C60" t="s">
         <v>0</v>
       </c>
       <c r="D60">
-        <v>20980</v>
+        <v>19480</v>
       </c>
       <c r="E60">
-        <v>20880</v>
+        <v>19380</v>
       </c>
       <c r="F60">
-        <v>19720</v>
+        <v>18500</v>
       </c>
       <c r="G60">
-        <v>16360</v>
+        <v>15470</v>
       </c>
       <c r="H60">
-        <v>16060</v>
+        <v>15170</v>
       </c>
     </row>
     <row r="61" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B61" s="1">
         <f t="shared" si="1"/>
-        <v>43815</v>
+        <v>43875</v>
       </c>
       <c r="C61" t="s">
         <v>1</v>
       </c>
       <c r="D61">
-        <v>21390</v>
+        <v>19860</v>
       </c>
       <c r="E61">
-        <v>21290</v>
+        <v>19760</v>
       </c>
       <c r="F61">
-        <v>20110</v>
+        <v>18870</v>
       </c>
       <c r="G61">
-        <v>16680</v>
+        <v>15770</v>
       </c>
       <c r="H61">
-        <v>16380</v>
+        <v>15470</v>
       </c>
     </row>
     <row r="62" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B62" s="1">
-        <v>43799</v>
+        <f t="shared" si="1"/>
+        <v>43860</v>
       </c>
       <c r="C62" t="s">
         <v>0</v>
       </c>
       <c r="D62">
-        <v>21170</v>
+        <v>20220</v>
       </c>
       <c r="E62">
-        <v>21070</v>
+        <v>20120</v>
       </c>
       <c r="F62">
-        <v>19810</v>
+        <v>19260</v>
       </c>
       <c r="G62">
-        <v>16280</v>
+        <v>16430</v>
       </c>
       <c r="H62">
-        <v>15980</v>
+        <v>16130</v>
       </c>
     </row>
     <row r="63" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B63" s="1">
-        <v>43799</v>
+        <f t="shared" si="1"/>
+        <v>43860</v>
       </c>
       <c r="C63" t="s">
         <v>1</v>
       </c>
       <c r="D63">
-        <v>21590</v>
+        <v>20620</v>
       </c>
       <c r="E63">
-        <v>21490</v>
+        <v>20520</v>
       </c>
       <c r="F63">
-        <v>20200</v>
+        <v>19640</v>
       </c>
       <c r="G63">
-        <v>16600</v>
+        <v>16750</v>
       </c>
       <c r="H63">
-        <v>16290</v>
+        <v>16450</v>
       </c>
     </row>
     <row r="64" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B64" s="1">
-        <f>B62-15</f>
-        <v>43784</v>
+        <f t="shared" si="1"/>
+        <v>43845</v>
       </c>
       <c r="C64" t="s">
         <v>0</v>
       </c>
       <c r="D64">
-        <v>20890</v>
+        <v>21010</v>
       </c>
       <c r="E64">
-        <v>20790</v>
+        <v>20910</v>
       </c>
       <c r="F64">
-        <v>19500</v>
+        <v>19840</v>
       </c>
       <c r="G64">
-        <v>16260</v>
+        <v>16840</v>
       </c>
       <c r="H64">
-        <v>15960</v>
+        <v>16540</v>
       </c>
     </row>
     <row r="65" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B65" s="1">
-        <f>B63-15</f>
-        <v>43784</v>
+        <f t="shared" si="1"/>
+        <v>43845</v>
       </c>
       <c r="C65" t="s">
         <v>1</v>
       </c>
       <c r="D65">
-        <v>21300</v>
+        <v>21430</v>
       </c>
       <c r="E65">
-        <v>21200</v>
+        <v>21320</v>
       </c>
       <c r="F65">
-        <v>19890</v>
+        <v>20230</v>
       </c>
       <c r="G65">
-        <v>16580</v>
+        <v>17170</v>
       </c>
       <c r="H65">
-        <v>16270</v>
+        <v>16870</v>
       </c>
     </row>
     <row r="66" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B66" s="1">
-        <f t="shared" ref="B66:B73" si="2">B64-15</f>
-        <v>43769</v>
+        <f t="shared" si="1"/>
+        <v>43830</v>
       </c>
       <c r="C66" t="s">
         <v>0</v>
       </c>
       <c r="D66">
-        <v>20540</v>
+        <v>21090</v>
       </c>
       <c r="E66">
-        <v>20440</v>
+        <v>20990</v>
       </c>
       <c r="F66">
-        <v>19250</v>
+        <v>19880</v>
       </c>
       <c r="G66">
-        <v>16350</v>
+        <v>16890</v>
       </c>
       <c r="H66">
-        <v>16050</v>
+        <v>16590</v>
       </c>
     </row>
     <row r="67" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B67" s="1">
+        <f t="shared" si="1"/>
+        <v>43830</v>
+      </c>
+      <c r="C67" t="s">
+        <v>1</v>
+      </c>
+      <c r="D67">
+        <v>21510</v>
+      </c>
+      <c r="E67">
+        <v>21400</v>
+      </c>
+      <c r="F67">
+        <v>20270</v>
+      </c>
+      <c r="G67">
+        <v>17220</v>
+      </c>
+      <c r="H67">
+        <v>16920</v>
+      </c>
+    </row>
+    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B68" s="1">
+        <f t="shared" si="1"/>
+        <v>43815</v>
+      </c>
+      <c r="C68" t="s">
+        <v>0</v>
+      </c>
+      <c r="D68">
+        <v>20980</v>
+      </c>
+      <c r="E68">
+        <v>20880</v>
+      </c>
+      <c r="F68">
+        <v>19720</v>
+      </c>
+      <c r="G68">
+        <v>16360</v>
+      </c>
+      <c r="H68">
+        <v>16060</v>
+      </c>
+    </row>
+    <row r="69" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B69" s="1">
+        <f t="shared" si="1"/>
+        <v>43815</v>
+      </c>
+      <c r="C69" t="s">
+        <v>1</v>
+      </c>
+      <c r="D69">
+        <v>21390</v>
+      </c>
+      <c r="E69">
+        <v>21290</v>
+      </c>
+      <c r="F69">
+        <v>20110</v>
+      </c>
+      <c r="G69">
+        <v>16680</v>
+      </c>
+      <c r="H69">
+        <v>16380</v>
+      </c>
+    </row>
+    <row r="70" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B70" s="1">
+        <v>43799</v>
+      </c>
+      <c r="C70" t="s">
+        <v>0</v>
+      </c>
+      <c r="D70">
+        <v>21170</v>
+      </c>
+      <c r="E70">
+        <v>21070</v>
+      </c>
+      <c r="F70">
+        <v>19810</v>
+      </c>
+      <c r="G70">
+        <v>16280</v>
+      </c>
+      <c r="H70">
+        <v>15980</v>
+      </c>
+    </row>
+    <row r="71" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B71" s="1">
+        <v>43799</v>
+      </c>
+      <c r="C71" t="s">
+        <v>1</v>
+      </c>
+      <c r="D71">
+        <v>21590</v>
+      </c>
+      <c r="E71">
+        <v>21490</v>
+      </c>
+      <c r="F71">
+        <v>20200</v>
+      </c>
+      <c r="G71">
+        <v>16600</v>
+      </c>
+      <c r="H71">
+        <v>16290</v>
+      </c>
+    </row>
+    <row r="72" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B72" s="1">
+        <f>B70-15</f>
+        <v>43784</v>
+      </c>
+      <c r="C72" t="s">
+        <v>0</v>
+      </c>
+      <c r="D72">
+        <v>20890</v>
+      </c>
+      <c r="E72">
+        <v>20790</v>
+      </c>
+      <c r="F72">
+        <v>19500</v>
+      </c>
+      <c r="G72">
+        <v>16260</v>
+      </c>
+      <c r="H72">
+        <v>15960</v>
+      </c>
+    </row>
+    <row r="73" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B73" s="1">
+        <f>B71-15</f>
+        <v>43784</v>
+      </c>
+      <c r="C73" t="s">
+        <v>1</v>
+      </c>
+      <c r="D73">
+        <v>21300</v>
+      </c>
+      <c r="E73">
+        <v>21200</v>
+      </c>
+      <c r="F73">
+        <v>19890</v>
+      </c>
+      <c r="G73">
+        <v>16580</v>
+      </c>
+      <c r="H73">
+        <v>16270</v>
+      </c>
+    </row>
+    <row r="74" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B74" s="1">
+        <f t="shared" ref="B74:B81" si="2">B72-15</f>
+        <v>43769</v>
+      </c>
+      <c r="C74" t="s">
+        <v>0</v>
+      </c>
+      <c r="D74">
+        <v>20540</v>
+      </c>
+      <c r="E74">
+        <v>20440</v>
+      </c>
+      <c r="F74">
+        <v>19250</v>
+      </c>
+      <c r="G74">
+        <v>16350</v>
+      </c>
+      <c r="H74">
+        <v>16050</v>
+      </c>
+    </row>
+    <row r="75" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B75" s="1">
         <f t="shared" si="2"/>
         <v>43769</v>
       </c>
-      <c r="C67" t="s">
-        <v>1</v>
-      </c>
-      <c r="D67">
+      <c r="C75" t="s">
+        <v>1</v>
+      </c>
+      <c r="D75">
         <v>20950</v>
       </c>
-      <c r="E67">
+      <c r="E75">
         <v>20840</v>
       </c>
-      <c r="F67">
+      <c r="F75">
         <v>19630</v>
       </c>
-      <c r="G67">
+      <c r="G75">
         <v>16670</v>
       </c>
-      <c r="H67">
+      <c r="H75">
         <v>16370</v>
       </c>
     </row>
-    <row r="68" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B68" s="1">
+    <row r="76" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B76" s="1">
         <f t="shared" si="2"/>
         <v>43754</v>
       </c>
-      <c r="C68" t="s">
-        <v>0</v>
-      </c>
-      <c r="D68">
+      <c r="C76" t="s">
+        <v>0</v>
+      </c>
+      <c r="D76">
         <v>20890</v>
       </c>
-      <c r="E68">
+      <c r="E76">
         <v>20790</v>
       </c>
-      <c r="F68">
+      <c r="F76">
         <v>19470</v>
       </c>
-      <c r="G68">
+      <c r="G76">
         <v>16520</v>
       </c>
-      <c r="H68">
+      <c r="H76">
         <v>16220</v>
       </c>
     </row>
-    <row r="69" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B69" s="1">
+    <row r="77" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B77" s="1">
         <f t="shared" si="2"/>
         <v>43754</v>
       </c>
-      <c r="C69" t="s">
-        <v>1</v>
-      </c>
-      <c r="D69">
+      <c r="C77" t="s">
+        <v>1</v>
+      </c>
+      <c r="D77">
         <v>21300</v>
       </c>
-      <c r="E69">
+      <c r="E77">
         <v>21200</v>
       </c>
-      <c r="F69">
+      <c r="F77">
         <v>19850</v>
       </c>
-      <c r="G69">
+      <c r="G77">
         <v>16850</v>
       </c>
-      <c r="H69">
+      <c r="H77">
         <v>16540</v>
       </c>
     </row>
-    <row r="70" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B70" s="1">
+    <row r="78" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B78" s="1">
         <f t="shared" si="2"/>
         <v>43739</v>
       </c>
-      <c r="C70" t="s">
-        <v>0</v>
-      </c>
-      <c r="D70">
+      <c r="C78" t="s">
+        <v>0</v>
+      </c>
+      <c r="D78">
         <v>21160</v>
       </c>
-      <c r="E70">
+      <c r="E78">
         <v>21060</v>
       </c>
-      <c r="F70">
+      <c r="F78">
         <v>19780</v>
       </c>
-      <c r="G70">
+      <c r="G78">
         <v>16930</v>
       </c>
-      <c r="H70">
+      <c r="H78">
         <v>16630</v>
       </c>
     </row>
-    <row r="71" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B71" s="1">
+    <row r="79" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B79" s="1">
         <f t="shared" si="2"/>
         <v>43739</v>
       </c>
-      <c r="C71" t="s">
-        <v>1</v>
-      </c>
-      <c r="D71">
+      <c r="C79" t="s">
+        <v>1</v>
+      </c>
+      <c r="D79">
         <v>21580</v>
       </c>
-      <c r="E71">
+      <c r="E79">
         <v>21480</v>
       </c>
-      <c r="F71">
+      <c r="F79">
         <v>20170</v>
       </c>
-      <c r="G71">
+      <c r="G79">
         <v>17260</v>
       </c>
-      <c r="H71">
+      <c r="H79">
         <v>16960</v>
       </c>
     </row>
-    <row r="72" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B72" s="1">
+    <row r="80" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B80" s="1">
         <f t="shared" si="2"/>
         <v>43724</v>
       </c>
-      <c r="C72" t="s">
-        <v>0</v>
-      </c>
-      <c r="D72">
+      <c r="C80" t="s">
+        <v>0</v>
+      </c>
+      <c r="D80">
         <v>20240</v>
       </c>
-      <c r="E72">
+      <c r="E80">
         <v>20140</v>
       </c>
-      <c r="F72">
+      <c r="F80">
         <v>19110</v>
       </c>
-      <c r="G72">
+      <c r="G80">
         <v>16500</v>
       </c>
-      <c r="H72">
+      <c r="H80">
         <v>16200</v>
       </c>
     </row>
-    <row r="73" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B73" s="1">
+    <row r="81" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B81" s="1">
         <f t="shared" si="2"/>
         <v>43724</v>
       </c>
-      <c r="C73" t="s">
-        <v>1</v>
-      </c>
-      <c r="D73">
+      <c r="C81" t="s">
+        <v>1</v>
+      </c>
+      <c r="D81">
         <v>20640</v>
       </c>
-      <c r="E73">
+      <c r="E81">
         <v>20540</v>
       </c>
-      <c r="F73">
+      <c r="F81">
         <v>19490</v>
       </c>
-      <c r="G73">
+      <c r="G81">
         <v>16830</v>
       </c>
-      <c r="H73">
+      <c r="H81">
         <v>16520</v>
-      </c>
-    </row>
-    <row r="74" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B74" s="1">
-        <v>43708</v>
-      </c>
-      <c r="C74" t="s">
-        <v>0</v>
-      </c>
-      <c r="D74">
-        <v>20330</v>
-      </c>
-      <c r="E74">
-        <v>20230</v>
-      </c>
-      <c r="F74">
-        <v>19220</v>
-      </c>
-      <c r="G74">
-        <v>16630</v>
-      </c>
-      <c r="H74">
-        <v>16330</v>
-      </c>
-    </row>
-    <row r="75" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B75" s="1">
-        <v>43708</v>
-      </c>
-      <c r="C75" t="s">
-        <v>1</v>
-      </c>
-      <c r="D75">
-        <v>20730</v>
-      </c>
-      <c r="E75">
-        <v>20630</v>
-      </c>
-      <c r="F75">
-        <v>19600</v>
-      </c>
-      <c r="G75">
-        <v>16960</v>
-      </c>
-      <c r="H75">
-        <v>16650</v>
-      </c>
-    </row>
-    <row r="76" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B76" s="1">
-        <v>43693</v>
-      </c>
-      <c r="C76" t="s">
-        <v>0</v>
-      </c>
-      <c r="D76">
-        <v>20500</v>
-      </c>
-      <c r="E76">
-        <v>20400</v>
-      </c>
-      <c r="F76">
-        <v>19350</v>
-      </c>
-      <c r="G76">
-        <v>16800</v>
-      </c>
-      <c r="H76">
-        <v>16500</v>
-      </c>
-    </row>
-    <row r="77" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B77" s="1">
-        <v>43693</v>
-      </c>
-      <c r="C77" t="s">
-        <v>1</v>
-      </c>
-      <c r="D77">
-        <v>20910</v>
-      </c>
-      <c r="E77">
-        <v>20800</v>
-      </c>
-      <c r="F77">
-        <v>19730</v>
-      </c>
-      <c r="G77">
-        <v>17130</v>
-      </c>
-      <c r="H77">
-        <v>16830</v>
-      </c>
-    </row>
-    <row r="78" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B78" s="1">
-        <v>43678</v>
-      </c>
-      <c r="C78" t="s">
-        <v>0</v>
-      </c>
-      <c r="D78">
-        <v>21010</v>
-      </c>
-      <c r="E78">
-        <v>20910</v>
-      </c>
-      <c r="F78">
-        <v>19900</v>
-      </c>
-      <c r="G78">
-        <v>17320</v>
-      </c>
-      <c r="H78">
-        <v>17020</v>
-      </c>
-    </row>
-    <row r="79" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B79" s="1">
-        <v>43678</v>
-      </c>
-      <c r="C79" t="s">
-        <v>1</v>
-      </c>
-      <c r="D79">
-        <v>21430</v>
-      </c>
-      <c r="E79">
-        <v>21320</v>
-      </c>
-      <c r="F79">
-        <v>20290</v>
-      </c>
-      <c r="G79">
-        <v>17660</v>
-      </c>
-      <c r="H79">
-        <v>17360</v>
-      </c>
-    </row>
-    <row r="80" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B80" s="1">
-        <f>B78-15</f>
-        <v>43663</v>
-      </c>
-      <c r="C80" t="s">
-        <v>0</v>
-      </c>
-      <c r="D80">
-        <v>21380</v>
-      </c>
-      <c r="E80">
-        <v>21230</v>
-      </c>
-      <c r="F80">
-        <v>20270</v>
-      </c>
-      <c r="G80">
-        <v>17290</v>
-      </c>
-      <c r="H80">
-        <v>16990</v>
-      </c>
-    </row>
-    <row r="81" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B81" s="1">
-        <f>B79-15</f>
-        <v>43663</v>
-      </c>
-      <c r="C81" t="s">
-        <v>1</v>
-      </c>
-      <c r="D81">
-        <v>21800</v>
-      </c>
-      <c r="E81">
-        <v>21650</v>
-      </c>
-      <c r="F81">
-        <v>20670</v>
-      </c>
-      <c r="G81">
-        <v>17630</v>
-      </c>
-      <c r="H81">
-        <v>17320</v>
       </c>
     </row>
     <row r="82" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B82" s="1">
-        <f t="shared" ref="B82:B97" si="3">B80-15</f>
-        <v>43648</v>
+        <v>43708</v>
       </c>
       <c r="C82" t="s">
         <v>0</v>
       </c>
       <c r="D82">
-        <v>20660</v>
+        <v>20330</v>
       </c>
       <c r="E82">
-        <v>20510</v>
+        <v>20230</v>
       </c>
       <c r="F82">
-        <v>19650</v>
+        <v>19220</v>
       </c>
       <c r="G82">
-        <v>17240</v>
+        <v>16630</v>
       </c>
       <c r="H82">
-        <v>16940</v>
+        <v>16330</v>
       </c>
     </row>
     <row r="83" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B83" s="1">
-        <f t="shared" si="3"/>
-        <v>43648</v>
+        <v>43708</v>
       </c>
       <c r="C83" t="s">
         <v>1</v>
       </c>
       <c r="D83">
-        <v>21070</v>
+        <v>20730</v>
       </c>
       <c r="E83">
-        <v>20920</v>
+        <v>20630</v>
       </c>
       <c r="F83">
-        <v>20040</v>
+        <v>19600</v>
       </c>
       <c r="G83">
-        <v>17580</v>
+        <v>16960</v>
       </c>
       <c r="H83">
-        <v>17270</v>
+        <v>16650</v>
       </c>
     </row>
     <row r="84" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B84" s="1">
-        <f t="shared" si="3"/>
-        <v>43633</v>
+        <v>43693</v>
       </c>
       <c r="C84" t="s">
         <v>0</v>
       </c>
       <c r="D84">
-        <v>20280</v>
+        <v>20500</v>
       </c>
       <c r="E84">
-        <v>20130</v>
+        <v>20400</v>
       </c>
       <c r="F84">
-        <v>19230</v>
+        <v>19350</v>
       </c>
       <c r="G84">
-        <v>16950</v>
+        <v>16800</v>
       </c>
       <c r="H84">
-        <v>16650</v>
+        <v>16500</v>
       </c>
     </row>
     <row r="85" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B85" s="1">
-        <f t="shared" si="3"/>
-        <v>43633</v>
+        <v>43693</v>
       </c>
       <c r="C85" t="s">
         <v>1</v>
       </c>
       <c r="D85">
-        <v>20680</v>
+        <v>20910</v>
       </c>
       <c r="E85">
-        <v>20530</v>
+        <v>20800</v>
       </c>
       <c r="F85">
-        <v>19610</v>
+        <v>19730</v>
       </c>
       <c r="G85">
-        <v>17280</v>
+        <v>17130</v>
       </c>
       <c r="H85">
-        <v>16980</v>
+        <v>16830</v>
       </c>
     </row>
     <row r="86" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B86" s="1">
-        <v>43617</v>
+        <v>43678</v>
       </c>
       <c r="C86" t="s">
         <v>0</v>
       </c>
       <c r="D86">
-        <v>21360</v>
+        <v>21010</v>
       </c>
       <c r="E86">
-        <v>21210</v>
+        <v>20910</v>
       </c>
       <c r="F86">
-        <v>20210</v>
+        <v>19900</v>
       </c>
       <c r="G86">
-        <v>17690</v>
+        <v>17320</v>
       </c>
       <c r="H86">
-        <v>17390</v>
+        <v>17020</v>
       </c>
     </row>
     <row r="87" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B87" s="1">
-        <v>43617</v>
+        <v>43678</v>
       </c>
       <c r="C87" t="s">
         <v>1</v>
       </c>
       <c r="D87">
-        <v>21780</v>
+        <v>21430</v>
       </c>
       <c r="E87">
-        <v>21630</v>
+        <v>21320</v>
       </c>
       <c r="F87">
-        <v>20610</v>
+        <v>20290</v>
       </c>
       <c r="G87">
-        <v>18040</v>
+        <v>17660</v>
       </c>
       <c r="H87">
-        <v>17730</v>
+        <v>17360</v>
       </c>
     </row>
     <row r="88" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B88" s="1">
-        <f t="shared" si="3"/>
-        <v>43602</v>
+        <f>B86-15</f>
+        <v>43663</v>
       </c>
       <c r="C88" t="s">
         <v>0</v>
       </c>
       <c r="D88">
-        <v>21740</v>
+        <v>21380</v>
       </c>
       <c r="E88">
-        <v>21590</v>
+        <v>21230</v>
       </c>
       <c r="F88">
-        <v>20480</v>
+        <v>20270</v>
       </c>
       <c r="G88">
-        <v>17910</v>
+        <v>17290</v>
       </c>
       <c r="H88">
-        <v>17610</v>
+        <v>16990</v>
       </c>
     </row>
     <row r="89" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B89" s="1">
-        <f t="shared" si="3"/>
-        <v>43602</v>
+        <f>B87-15</f>
+        <v>43663</v>
       </c>
       <c r="C89" t="s">
         <v>1</v>
       </c>
       <c r="D89">
-        <v>22170</v>
+        <v>21800</v>
       </c>
       <c r="E89">
-        <v>22020</v>
+        <v>21650</v>
       </c>
       <c r="F89">
-        <v>20880</v>
+        <v>20670</v>
       </c>
       <c r="G89">
-        <v>18260</v>
+        <v>17630</v>
       </c>
       <c r="H89">
-        <v>17960</v>
+        <v>17320</v>
       </c>
     </row>
     <row r="90" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B90" s="1">
-        <f t="shared" si="3"/>
-        <v>43587</v>
+        <f t="shared" ref="B90:B105" si="3">B88-15</f>
+        <v>43648</v>
       </c>
       <c r="C90" t="s">
         <v>0</v>
       </c>
       <c r="D90">
-        <v>22340</v>
+        <v>20660</v>
       </c>
       <c r="E90">
-        <v>22190</v>
+        <v>20510</v>
       </c>
       <c r="F90">
-        <v>20680</v>
+        <v>19650</v>
       </c>
       <c r="G90">
-        <v>17990</v>
+        <v>17240</v>
       </c>
       <c r="H90">
-        <v>17690</v>
+        <v>16940</v>
       </c>
     </row>
     <row r="91" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B91" s="1">
         <f t="shared" si="3"/>
-        <v>43587</v>
+        <v>43648</v>
       </c>
       <c r="C91" t="s">
         <v>1</v>
       </c>
       <c r="D91">
-        <v>22780</v>
+        <v>21070</v>
       </c>
       <c r="E91">
-        <v>22630</v>
+        <v>20920</v>
       </c>
       <c r="F91">
-        <v>21090</v>
+        <v>20040</v>
       </c>
       <c r="G91">
-        <v>18340</v>
+        <v>17580</v>
       </c>
       <c r="H91">
-        <v>18040</v>
+        <v>17270</v>
       </c>
     </row>
     <row r="92" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B92" s="1">
         <f t="shared" si="3"/>
-        <v>43572</v>
+        <v>43633</v>
       </c>
       <c r="C92" t="s">
         <v>0</v>
       </c>
       <c r="D92">
-        <v>21380</v>
+        <v>20280</v>
       </c>
       <c r="E92">
-        <v>21230</v>
+        <v>20130</v>
       </c>
       <c r="F92">
-        <v>19700</v>
+        <v>19230</v>
       </c>
       <c r="G92">
-        <v>17680</v>
+        <v>16950</v>
       </c>
       <c r="H92">
-        <v>17380</v>
+        <v>16650</v>
       </c>
     </row>
     <row r="93" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B93" s="1">
         <f t="shared" si="3"/>
-        <v>43572</v>
+        <v>43633</v>
       </c>
       <c r="C93" t="s">
         <v>1</v>
       </c>
       <c r="D93">
-        <v>21800</v>
+        <v>20680</v>
       </c>
       <c r="E93">
-        <v>21650</v>
+        <v>20530</v>
       </c>
       <c r="F93">
-        <v>20090</v>
+        <v>19610</v>
       </c>
       <c r="G93">
-        <v>18030</v>
+        <v>17280</v>
       </c>
       <c r="H93">
-        <v>17720</v>
+        <v>16980</v>
       </c>
     </row>
     <row r="94" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B94" s="1">
-        <f t="shared" si="3"/>
-        <v>43557</v>
+        <v>43617</v>
       </c>
       <c r="C94" t="s">
         <v>0</v>
       </c>
       <c r="D94">
-        <v>20180</v>
+        <v>21360</v>
       </c>
       <c r="E94">
-        <v>20030</v>
+        <v>21210</v>
       </c>
       <c r="F94">
-        <v>18580</v>
+        <v>20210</v>
       </c>
       <c r="G94">
-        <v>17380</v>
+        <v>17690</v>
       </c>
       <c r="H94">
-        <v>17080</v>
+        <v>17390</v>
       </c>
     </row>
     <row r="95" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B95" s="1">
-        <f t="shared" si="3"/>
-        <v>43557</v>
+        <v>43617</v>
       </c>
       <c r="C95" t="s">
         <v>1</v>
       </c>
       <c r="D95">
-        <v>20580</v>
+        <v>21780</v>
       </c>
       <c r="E95">
-        <v>20430</v>
+        <v>21630</v>
       </c>
       <c r="F95">
-        <v>18950</v>
+        <v>20610</v>
       </c>
       <c r="G95">
-        <v>17720</v>
+        <v>18040</v>
       </c>
       <c r="H95">
-        <v>17420</v>
+        <v>17730</v>
       </c>
     </row>
     <row r="96" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B96" s="1">
         <f t="shared" si="3"/>
-        <v>43542</v>
+        <v>43602</v>
       </c>
       <c r="C96" t="s">
         <v>0</v>
       </c>
       <c r="D96">
-        <v>18690</v>
+        <v>21740</v>
       </c>
       <c r="E96">
-        <v>18540</v>
+        <v>21590</v>
       </c>
       <c r="F96">
-        <v>17210</v>
+        <v>20480</v>
       </c>
       <c r="G96">
-        <v>16060</v>
+        <v>17910</v>
       </c>
       <c r="H96">
-        <v>15860</v>
+        <v>17610</v>
       </c>
     </row>
     <row r="97" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B97" s="1">
         <f t="shared" si="3"/>
-        <v>43542</v>
+        <v>43602</v>
       </c>
       <c r="C97" t="s">
         <v>1</v>
       </c>
       <c r="D97">
-        <v>19060</v>
+        <v>22170</v>
       </c>
       <c r="E97">
-        <v>18910</v>
+        <v>22020</v>
       </c>
       <c r="F97">
-        <v>17550</v>
+        <v>20880</v>
       </c>
       <c r="G97">
-        <v>16380</v>
+        <v>18260</v>
       </c>
       <c r="H97">
-        <v>16170</v>
+        <v>17960</v>
       </c>
     </row>
     <row r="98" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B98" s="1">
-        <f>B96-15</f>
-        <v>43527</v>
+        <f t="shared" si="3"/>
+        <v>43587</v>
       </c>
       <c r="C98" t="s">
         <v>0</v>
       </c>
       <c r="D98">
-        <v>18690</v>
+        <v>22340</v>
       </c>
       <c r="E98">
-        <v>18540</v>
+        <v>22190</v>
       </c>
       <c r="F98">
-        <v>17210</v>
+        <v>20680</v>
       </c>
       <c r="G98">
-        <v>16060</v>
+        <v>17990</v>
       </c>
       <c r="H98">
-        <v>15860</v>
+        <v>17690</v>
       </c>
     </row>
     <row r="99" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B99" s="1">
-        <f>B97-15</f>
-        <v>43527</v>
+        <f t="shared" si="3"/>
+        <v>43587</v>
       </c>
       <c r="C99" t="s">
         <v>1</v>
       </c>
       <c r="D99">
-        <v>19060</v>
+        <v>22780</v>
       </c>
       <c r="E99">
-        <v>18910</v>
+        <v>22630</v>
       </c>
       <c r="F99">
-        <v>17550</v>
+        <v>21090</v>
       </c>
       <c r="G99">
-        <v>16380</v>
+        <v>18340</v>
       </c>
       <c r="H99">
-        <v>16170</v>
+        <v>18040</v>
       </c>
     </row>
     <row r="100" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B100" s="1">
-        <v>43511</v>
+        <f t="shared" si="3"/>
+        <v>43572</v>
       </c>
       <c r="C100" t="s">
         <v>0</v>
       </c>
       <c r="D100">
-        <v>17750</v>
+        <v>21380</v>
       </c>
       <c r="E100">
-        <v>17600</v>
+        <v>21230</v>
       </c>
       <c r="F100">
-        <v>16270</v>
+        <v>19700</v>
       </c>
       <c r="G100">
-        <v>15100</v>
+        <v>17680</v>
       </c>
       <c r="H100">
-        <v>14900</v>
+        <v>17380</v>
       </c>
     </row>
     <row r="101" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B101" s="1">
-        <v>43511</v>
+        <f t="shared" si="3"/>
+        <v>43572</v>
       </c>
       <c r="C101" t="s">
         <v>1</v>
       </c>
       <c r="D101">
-        <v>18100</v>
+        <v>21800</v>
       </c>
       <c r="E101">
-        <v>17950</v>
+        <v>21650</v>
       </c>
       <c r="F101">
-        <v>16590</v>
+        <v>20090</v>
       </c>
       <c r="G101">
-        <v>15400</v>
+        <v>18030</v>
       </c>
       <c r="H101">
-        <v>15190</v>
+        <v>17720</v>
       </c>
     </row>
     <row r="102" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B102" s="1">
-        <f t="shared" ref="B102:B103" si="4">B100-15</f>
-        <v>43496</v>
+        <f t="shared" si="3"/>
+        <v>43557</v>
       </c>
       <c r="C102" t="s">
         <v>0</v>
       </c>
       <c r="D102">
-        <v>17750</v>
+        <v>20180</v>
       </c>
       <c r="E102">
-        <v>17600</v>
+        <v>20030</v>
       </c>
       <c r="F102">
-        <v>16270</v>
+        <v>18580</v>
       </c>
       <c r="G102">
-        <v>15100</v>
+        <v>17380</v>
       </c>
       <c r="H102">
-        <v>14900</v>
+        <v>17080</v>
       </c>
     </row>
     <row r="103" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B103" s="1">
-        <f t="shared" si="4"/>
-        <v>43496</v>
+        <f t="shared" si="3"/>
+        <v>43557</v>
       </c>
       <c r="C103" t="s">
         <v>1</v>
       </c>
       <c r="D103">
-        <v>18100</v>
+        <v>20580</v>
       </c>
       <c r="E103">
-        <v>17950</v>
+        <v>20430</v>
       </c>
       <c r="F103">
-        <v>16590</v>
+        <v>18950</v>
       </c>
       <c r="G103">
-        <v>15400</v>
+        <v>17720</v>
       </c>
       <c r="H103">
-        <v>15190</v>
+        <v>17420</v>
       </c>
     </row>
     <row r="104" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B104" s="1">
-        <f>B102-15</f>
-        <v>43481</v>
+        <f t="shared" si="3"/>
+        <v>43542</v>
       </c>
       <c r="C104" t="s">
         <v>0</v>
       </c>
       <c r="D104">
-        <v>17750</v>
+        <v>18690</v>
       </c>
       <c r="E104">
-        <v>17600</v>
+        <v>18540</v>
       </c>
       <c r="F104">
-        <v>16270</v>
+        <v>17210</v>
       </c>
       <c r="G104">
-        <v>15050</v>
+        <v>16060</v>
       </c>
       <c r="H104">
-        <v>14900</v>
+        <v>15860</v>
       </c>
     </row>
     <row r="105" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B105" s="1">
-        <f>B103-15</f>
-        <v>43481</v>
+        <f t="shared" si="3"/>
+        <v>43542</v>
       </c>
       <c r="C105" t="s">
         <v>1</v>
       </c>
       <c r="D105">
-        <v>18100</v>
+        <v>19060</v>
       </c>
       <c r="E105">
-        <v>17950</v>
+        <v>18910</v>
       </c>
       <c r="F105">
-        <v>16590</v>
+        <v>17550</v>
       </c>
       <c r="G105">
-        <v>15350</v>
+        <v>16380</v>
       </c>
       <c r="H105">
-        <v>15190</v>
+        <v>16170</v>
       </c>
     </row>
     <row r="106" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B106" s="1">
-        <f t="shared" ref="B106" si="5">B104-15</f>
-        <v>43466</v>
+        <f>B104-15</f>
+        <v>43527</v>
       </c>
       <c r="C106" t="s">
         <v>0</v>
       </c>
       <c r="D106">
-        <v>17750</v>
+        <v>18690</v>
       </c>
       <c r="E106">
-        <v>17600</v>
+        <v>18540</v>
       </c>
       <c r="F106">
-        <v>16270</v>
+        <v>17210</v>
       </c>
       <c r="G106">
-        <v>15050</v>
+        <v>16060</v>
       </c>
       <c r="H106">
-        <v>14900</v>
+        <v>15860</v>
       </c>
     </row>
     <row r="107" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B107" s="1">
         <f>B105-15</f>
-        <v>43466</v>
+        <v>43527</v>
       </c>
       <c r="C107" t="s">
         <v>1</v>
       </c>
       <c r="D107">
-        <v>18100</v>
+        <v>19060</v>
       </c>
       <c r="E107">
-        <v>17950</v>
+        <v>18910</v>
       </c>
       <c r="F107">
-        <v>16590</v>
+        <v>17550</v>
       </c>
       <c r="G107">
-        <v>15350</v>
+        <v>16380</v>
       </c>
       <c r="H107">
-        <v>15190</v>
+        <v>16170</v>
       </c>
     </row>
     <row r="108" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B108" s="1">
-        <v>43455</v>
+        <v>43511</v>
       </c>
       <c r="C108" t="s">
         <v>0</v>
       </c>
       <c r="D108">
-        <v>18290</v>
+        <v>17750</v>
       </c>
       <c r="E108">
-        <v>18140</v>
+        <v>17600</v>
       </c>
       <c r="F108">
-        <v>16780</v>
+        <v>16270</v>
       </c>
       <c r="G108">
-        <v>16150</v>
+        <v>15100</v>
       </c>
       <c r="H108">
-        <v>16000</v>
+        <v>14900</v>
       </c>
     </row>
     <row r="109" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B109" s="1">
-        <v>43455</v>
+        <v>43511</v>
       </c>
       <c r="C109" t="s">
         <v>1</v>
       </c>
       <c r="D109">
-        <v>18650</v>
+        <v>18100</v>
       </c>
       <c r="E109">
-        <v>18500</v>
+        <v>17950</v>
       </c>
       <c r="F109">
-        <v>17110</v>
+        <v>16590</v>
       </c>
       <c r="G109">
-        <v>16470</v>
+        <v>15400</v>
       </c>
       <c r="H109">
-        <v>16320</v>
+        <v>15190</v>
       </c>
     </row>
     <row r="110" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B110" s="1">
-        <f>B108-15</f>
-        <v>43440</v>
+        <f t="shared" ref="B110:B111" si="4">B108-15</f>
+        <v>43496</v>
       </c>
       <c r="C110" t="s">
         <v>0</v>
       </c>
       <c r="D110">
-        <v>18600</v>
+        <v>17750</v>
       </c>
       <c r="E110">
-        <v>18450</v>
+        <v>17600</v>
       </c>
       <c r="F110">
-        <v>17180</v>
+        <v>16270</v>
       </c>
       <c r="G110">
-        <v>16400</v>
+        <v>15100</v>
       </c>
       <c r="H110">
-        <v>16250</v>
+        <v>14900</v>
       </c>
     </row>
     <row r="111" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B111" s="1">
-        <f>B109-15</f>
-        <v>43440</v>
+        <f t="shared" si="4"/>
+        <v>43496</v>
       </c>
       <c r="C111" t="s">
         <v>1</v>
       </c>
       <c r="D111">
-        <v>18970</v>
+        <v>18100</v>
       </c>
       <c r="E111">
-        <v>18810</v>
+        <v>17950</v>
       </c>
       <c r="F111">
-        <v>17520</v>
+        <v>16590</v>
       </c>
       <c r="G111">
-        <v>16720</v>
+        <v>15400</v>
       </c>
       <c r="H111">
-        <v>16570</v>
+        <v>15190</v>
       </c>
     </row>
     <row r="112" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B112" s="1">
-        <f t="shared" ref="B112:B175" si="6">B110-15</f>
-        <v>43425</v>
+        <f>B110-15</f>
+        <v>43481</v>
       </c>
       <c r="C112" t="s">
         <v>0</v>
       </c>
       <c r="D112">
-        <v>20120</v>
+        <v>17750</v>
       </c>
       <c r="E112">
-        <v>19970</v>
+        <v>17600</v>
       </c>
       <c r="F112">
-        <v>18620</v>
+        <v>16270</v>
       </c>
       <c r="G112">
-        <v>17780</v>
+        <v>15050</v>
       </c>
       <c r="H112">
-        <v>17630</v>
+        <v>14900</v>
       </c>
     </row>
     <row r="113" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B113" s="1">
-        <f t="shared" si="6"/>
-        <v>43425</v>
+        <f>B111-15</f>
+        <v>43481</v>
       </c>
       <c r="C113" t="s">
         <v>1</v>
       </c>
       <c r="D113">
-        <v>20520</v>
+        <v>18100</v>
       </c>
       <c r="E113">
-        <v>20360</v>
+        <v>17950</v>
       </c>
       <c r="F113">
-        <v>18990</v>
+        <v>16590</v>
       </c>
       <c r="G113">
-        <v>18130</v>
+        <v>15350</v>
       </c>
       <c r="H113">
-        <v>17980</v>
+        <v>15190</v>
       </c>
     </row>
     <row r="114" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B114" s="1">
-        <f t="shared" si="6"/>
-        <v>43410</v>
+        <f t="shared" ref="B114" si="5">B112-15</f>
+        <v>43466</v>
       </c>
       <c r="C114" t="s">
         <v>0</v>
       </c>
       <c r="D114">
-        <v>21210</v>
+        <v>17750</v>
       </c>
       <c r="E114">
-        <v>21060</v>
+        <v>17600</v>
       </c>
       <c r="F114">
-        <v>19600</v>
+        <v>16270</v>
       </c>
       <c r="G114">
-        <v>18640</v>
+        <v>15050</v>
       </c>
       <c r="H114">
-        <v>18540</v>
+        <v>14900</v>
       </c>
     </row>
     <row r="115" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B115" s="1">
-        <f t="shared" si="6"/>
-        <v>43410</v>
+        <f>B113-15</f>
+        <v>43466</v>
       </c>
       <c r="C115" t="s">
         <v>1</v>
       </c>
       <c r="D115">
-        <v>21630</v>
+        <v>18100</v>
       </c>
       <c r="E115">
-        <v>21480</v>
+        <v>17950</v>
       </c>
       <c r="F115">
-        <v>19990</v>
+        <v>16590</v>
       </c>
       <c r="G115">
-        <v>19010</v>
+        <v>15350</v>
       </c>
       <c r="H115">
-        <v>18910</v>
+        <v>15190</v>
       </c>
     </row>
     <row r="116" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B116" s="1">
-        <f t="shared" si="6"/>
-        <v>43395</v>
+        <v>43455</v>
       </c>
       <c r="C116" t="s">
         <v>0</v>
       </c>
       <c r="D116">
-        <v>22350</v>
+        <v>18290</v>
       </c>
       <c r="E116">
-        <v>22200</v>
+        <v>18140</v>
       </c>
       <c r="F116">
-        <v>20680</v>
+        <v>16780</v>
       </c>
       <c r="G116">
-        <v>18710</v>
+        <v>16150</v>
       </c>
       <c r="H116">
-        <v>18610</v>
+        <v>16000</v>
       </c>
     </row>
     <row r="117" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B117" s="1">
-        <f t="shared" si="6"/>
-        <v>43395</v>
+        <v>43455</v>
       </c>
       <c r="C117" t="s">
         <v>1</v>
       </c>
       <c r="D117">
-        <v>22790</v>
+        <v>18650</v>
       </c>
       <c r="E117">
-        <v>22640</v>
+        <v>18500</v>
       </c>
       <c r="F117">
-        <v>21090</v>
+        <v>17110</v>
       </c>
       <c r="G117">
-        <v>19080</v>
+        <v>16470</v>
       </c>
       <c r="H117">
-        <v>19080</v>
+        <v>16320</v>
       </c>
     </row>
     <row r="118" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B118" s="1">
-        <v>43379</v>
+        <f>B116-15</f>
+        <v>43440</v>
       </c>
       <c r="C118" t="s">
         <v>0</v>
       </c>
       <c r="D118">
-        <v>22490</v>
+        <v>18600</v>
       </c>
       <c r="E118">
-        <v>22340</v>
+        <v>18450</v>
       </c>
       <c r="F118">
-        <v>20900</v>
+        <v>17180</v>
       </c>
       <c r="G118">
-        <v>18710</v>
+        <v>16400</v>
       </c>
       <c r="H118">
-        <v>18610</v>
+        <v>16250</v>
       </c>
     </row>
     <row r="119" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B119" s="1">
-        <v>43379</v>
+        <f>B117-15</f>
+        <v>43440</v>
       </c>
       <c r="C119" t="s">
         <v>1</v>
       </c>
       <c r="D119">
-        <v>22930</v>
+        <v>18970</v>
       </c>
       <c r="E119">
-        <v>22780</v>
+        <v>18810</v>
       </c>
       <c r="F119">
-        <v>21310</v>
+        <v>17520</v>
       </c>
       <c r="G119">
-        <v>19080</v>
+        <v>16720</v>
       </c>
       <c r="H119">
-        <v>19080</v>
+        <v>16570</v>
       </c>
     </row>
     <row r="120" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B120" s="1">
-        <f t="shared" si="6"/>
-        <v>43364</v>
+        <f t="shared" ref="B120:B131" si="6">B118-15</f>
+        <v>43425</v>
       </c>
       <c r="C120" t="s">
         <v>0</v>
       </c>
       <c r="D120">
-        <v>21920</v>
+        <v>20120</v>
       </c>
       <c r="E120">
-        <v>21770</v>
+        <v>19970</v>
       </c>
       <c r="F120">
-        <v>20230</v>
+        <v>18620</v>
       </c>
       <c r="G120">
-        <v>18220</v>
+        <v>17780</v>
       </c>
       <c r="H120">
-        <v>18120</v>
+        <v>17630</v>
       </c>
     </row>
     <row r="121" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B121" s="1">
         <f t="shared" si="6"/>
-        <v>43364</v>
+        <v>43425</v>
       </c>
       <c r="C121" t="s">
         <v>1</v>
       </c>
       <c r="D121">
-        <v>22350</v>
+        <v>20520</v>
       </c>
       <c r="E121">
-        <v>22200</v>
+        <v>20360</v>
       </c>
       <c r="F121">
-        <v>20630</v>
+        <v>18990</v>
       </c>
       <c r="G121">
-        <v>18580</v>
+        <v>18130</v>
       </c>
       <c r="H121">
-        <v>18480</v>
+        <v>17980</v>
       </c>
     </row>
     <row r="122" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B122" s="1">
         <f t="shared" si="6"/>
-        <v>43349</v>
+        <v>43410</v>
       </c>
       <c r="C122" t="s">
         <v>0</v>
       </c>
       <c r="D122">
-        <v>21620</v>
+        <v>21210</v>
       </c>
       <c r="E122">
-        <v>21470</v>
+        <v>21060</v>
       </c>
       <c r="F122">
-        <v>19910</v>
+        <v>19600</v>
       </c>
       <c r="G122">
-        <v>18160</v>
+        <v>18640</v>
       </c>
       <c r="H122">
-        <v>18060</v>
+        <v>18540</v>
       </c>
     </row>
     <row r="123" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B123" s="1">
         <f t="shared" si="6"/>
+        <v>43410</v>
+      </c>
+      <c r="C123" t="s">
+        <v>1</v>
+      </c>
+      <c r="D123">
+        <v>21630</v>
+      </c>
+      <c r="E123">
+        <v>21480</v>
+      </c>
+      <c r="F123">
+        <v>19990</v>
+      </c>
+      <c r="G123">
+        <v>19010</v>
+      </c>
+      <c r="H123">
+        <v>18910</v>
+      </c>
+    </row>
+    <row r="124" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B124" s="1">
+        <f t="shared" si="6"/>
+        <v>43395</v>
+      </c>
+      <c r="C124" t="s">
+        <v>0</v>
+      </c>
+      <c r="D124">
+        <v>22350</v>
+      </c>
+      <c r="E124">
+        <v>22200</v>
+      </c>
+      <c r="F124">
+        <v>20680</v>
+      </c>
+      <c r="G124">
+        <v>18710</v>
+      </c>
+      <c r="H124">
+        <v>18610</v>
+      </c>
+    </row>
+    <row r="125" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B125" s="1">
+        <f t="shared" si="6"/>
+        <v>43395</v>
+      </c>
+      <c r="C125" t="s">
+        <v>1</v>
+      </c>
+      <c r="D125">
+        <v>22790</v>
+      </c>
+      <c r="E125">
+        <v>22640</v>
+      </c>
+      <c r="F125">
+        <v>21090</v>
+      </c>
+      <c r="G125">
+        <v>19080</v>
+      </c>
+      <c r="H125">
+        <v>19080</v>
+      </c>
+    </row>
+    <row r="126" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B126" s="1">
+        <v>43379</v>
+      </c>
+      <c r="C126" t="s">
+        <v>0</v>
+      </c>
+      <c r="D126">
+        <v>22490</v>
+      </c>
+      <c r="E126">
+        <v>22340</v>
+      </c>
+      <c r="F126">
+        <v>20900</v>
+      </c>
+      <c r="G126">
+        <v>18710</v>
+      </c>
+      <c r="H126">
+        <v>18610</v>
+      </c>
+    </row>
+    <row r="127" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B127" s="1">
+        <v>43379</v>
+      </c>
+      <c r="C127" t="s">
+        <v>1</v>
+      </c>
+      <c r="D127">
+        <v>22930</v>
+      </c>
+      <c r="E127">
+        <v>22780</v>
+      </c>
+      <c r="F127">
+        <v>21310</v>
+      </c>
+      <c r="G127">
+        <v>19080</v>
+      </c>
+      <c r="H127">
+        <v>19080</v>
+      </c>
+    </row>
+    <row r="128" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B128" s="1">
+        <f t="shared" si="6"/>
+        <v>43364</v>
+      </c>
+      <c r="C128" t="s">
+        <v>0</v>
+      </c>
+      <c r="D128">
+        <v>21920</v>
+      </c>
+      <c r="E128">
+        <v>21770</v>
+      </c>
+      <c r="F128">
+        <v>20230</v>
+      </c>
+      <c r="G128">
+        <v>18220</v>
+      </c>
+      <c r="H128">
+        <v>18120</v>
+      </c>
+    </row>
+    <row r="129" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B129" s="1">
+        <f t="shared" si="6"/>
+        <v>43364</v>
+      </c>
+      <c r="C129" t="s">
+        <v>1</v>
+      </c>
+      <c r="D129">
+        <v>22350</v>
+      </c>
+      <c r="E129">
+        <v>22200</v>
+      </c>
+      <c r="F129">
+        <v>20630</v>
+      </c>
+      <c r="G129">
+        <v>18580</v>
+      </c>
+      <c r="H129">
+        <v>18480</v>
+      </c>
+    </row>
+    <row r="130" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B130" s="1">
+        <f t="shared" si="6"/>
         <v>43349</v>
       </c>
-      <c r="C123" t="s">
-        <v>1</v>
-      </c>
-      <c r="D123">
+      <c r="C130" t="s">
+        <v>0</v>
+      </c>
+      <c r="D130">
+        <v>21620</v>
+      </c>
+      <c r="E130">
+        <v>21470</v>
+      </c>
+      <c r="F130">
+        <v>19910</v>
+      </c>
+      <c r="G130">
+        <v>18160</v>
+      </c>
+      <c r="H130">
+        <v>18060</v>
+      </c>
+    </row>
+    <row r="131" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B131" s="1">
+        <f t="shared" si="6"/>
+        <v>43349</v>
+      </c>
+      <c r="C131" t="s">
+        <v>1</v>
+      </c>
+      <c r="D131">
         <v>22050</v>
       </c>
-      <c r="E123">
+      <c r="E131">
         <v>21890</v>
       </c>
-      <c r="F123">
+      <c r="F131">
         <v>20300</v>
       </c>
-      <c r="G123">
+      <c r="G131">
         <v>18520</v>
       </c>
-      <c r="H123">
+      <c r="H131">
         <v>18420</v>
       </c>
     </row>

</xml_diff>